<commit_message>
fixed PLC logic for red line and updated wayside jurisdiction in excel
</commit_message>
<xml_diff>
--- a/src/main/TrackController/redLine.xlsx
+++ b/src/main/TrackController/redLine.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quiqu\Desktop\ECE1140\ECE-1140\src\main\TrackController\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asher\Desktop\Trains\src\main\TrackController\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59ABE059-6378-403B-A506-3041880E3717}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B44A048B-F8E1-4E8C-B40F-5C9CD616CB72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Red_Info" sheetId="8" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="46">
   <si>
     <t>Block Number</t>
   </si>
@@ -548,21 +548,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FCA0872-F3C1-4B8E-B7BD-13508CAEC5E4}">
-  <dimension ref="A1:E77"/>
+  <dimension ref="A1:E79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="120" zoomScaleNormal="101" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="101" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.5546875" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="52.77734375" customWidth="1"/>
+    <col min="1" max="1" width="13.5703125" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>24</v>
       </c>
@@ -579,7 +579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>43</v>
       </c>
@@ -587,7 +587,7 @@
         <v>45</v>
       </c>
       <c r="C2" s="4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>31</v>
@@ -596,55 +596,56 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="str">
-        <f>A2</f>
-        <v>wayside1R</v>
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="B3" s="2">
         <v>45</v>
       </c>
-      <c r="C3" s="2">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2"/>
+      <c r="C3" s="4">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
-        <f t="shared" ref="A4:A67" si="0">A3</f>
+        <f>A3</f>
         <v>wayside1R</v>
       </c>
       <c r="B4" s="2">
         <v>45</v>
       </c>
       <c r="C4" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="A5:A68" si="0">A4</f>
         <v>wayside1R</v>
       </c>
       <c r="B5" s="2">
         <v>45</v>
       </c>
-      <c r="C5" s="4">
-        <v>4</v>
+      <c r="C5" s="2">
+        <v>3</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside1R</v>
@@ -652,15 +653,15 @@
       <c r="B6" s="2">
         <v>45</v>
       </c>
-      <c r="C6" s="2">
-        <v>5</v>
+      <c r="C6" s="4">
+        <v>4</v>
       </c>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside1R</v>
@@ -669,14 +670,14 @@
         <v>45</v>
       </c>
       <c r="C7" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside1R</v>
@@ -684,17 +685,15 @@
       <c r="B8" s="2">
         <v>45</v>
       </c>
-      <c r="C8" s="4">
-        <v>7</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>26</v>
-      </c>
+      <c r="C8" s="2">
+        <v>6</v>
+      </c>
+      <c r="D8" s="2"/>
       <c r="E8" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside1R</v>
@@ -702,15 +701,17 @@
       <c r="B9" s="2">
         <v>45</v>
       </c>
-      <c r="C9" s="2">
-        <v>8</v>
-      </c>
-      <c r="D9" s="2"/>
+      <c r="C9" s="4">
+        <v>7</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="E9" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside1R</v>
@@ -719,16 +720,14 @@
         <v>45</v>
       </c>
       <c r="C10" s="2">
-        <v>9</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>32</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D10" s="2"/>
       <c r="E10" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside1R</v>
@@ -736,17 +735,17 @@
       <c r="B11" s="2">
         <v>45</v>
       </c>
-      <c r="C11" s="4">
-        <v>10</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>31</v>
+      <c r="C11" s="2">
+        <v>9</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside1R</v>
@@ -754,15 +753,17 @@
       <c r="B12" s="2">
         <v>45</v>
       </c>
-      <c r="C12" s="2">
-        <v>11</v>
-      </c>
-      <c r="D12" s="2"/>
+      <c r="C12" s="4">
+        <v>10</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="E12" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside1R</v>
@@ -770,31 +771,31 @@
       <c r="B13" s="2">
         <v>45</v>
       </c>
-      <c r="C13" s="4">
-        <v>12</v>
+      <c r="C13" s="2">
+        <v>11</v>
       </c>
       <c r="D13" s="2"/>
       <c r="E13" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside1R</v>
       </c>
       <c r="B14" s="2">
-        <v>70</v>
-      </c>
-      <c r="C14" s="2">
-        <v>13</v>
+        <v>45</v>
+      </c>
+      <c r="C14" s="4">
+        <v>12</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside1R</v>
@@ -803,14 +804,14 @@
         <v>70</v>
       </c>
       <c r="C15" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" s="2"/>
       <c r="E15" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside1R</v>
@@ -818,17 +819,15 @@
       <c r="B16" s="2">
         <v>70</v>
       </c>
-      <c r="C16" s="4">
-        <v>15</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>31</v>
-      </c>
+      <c r="C16" s="2">
+        <v>14</v>
+      </c>
+      <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside1R</v>
@@ -836,33 +835,35 @@
       <c r="B17" s="2">
         <v>70</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="4">
+        <v>15</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>wayside1R</v>
+      </c>
+      <c r="B18" s="2">
+        <v>70</v>
+      </c>
+      <c r="C18" s="2">
         <v>16</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>wayside1R</v>
-      </c>
-      <c r="B18" s="2">
-        <v>60</v>
-      </c>
-      <c r="C18" s="4">
-        <v>17</v>
-      </c>
-      <c r="D18" s="2"/>
       <c r="E18" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside1R</v>
@@ -870,15 +871,15 @@
       <c r="B19" s="2">
         <v>60</v>
       </c>
-      <c r="C19" s="2">
-        <v>18</v>
+      <c r="C19" s="4">
+        <v>17</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside1R</v>
@@ -887,14 +888,14 @@
         <v>60</v>
       </c>
       <c r="C20" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D20" s="2"/>
       <c r="E20" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside1R</v>
@@ -902,33 +903,31 @@
       <c r="B21" s="2">
         <v>60</v>
       </c>
-      <c r="C21" s="4">
-        <v>20</v>
+      <c r="C21" s="2">
+        <v>19</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside1R</v>
       </c>
       <c r="B22" s="2">
-        <v>70</v>
-      </c>
-      <c r="C22" s="2">
-        <v>21</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>27</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C22" s="4">
+        <v>20</v>
+      </c>
+      <c r="D22" s="2"/>
       <c r="E22" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside1R</v>
@@ -936,15 +935,17 @@
       <c r="B23" s="2">
         <v>70</v>
       </c>
-      <c r="C23" s="4">
-        <v>22</v>
-      </c>
-      <c r="D23" s="2"/>
+      <c r="C23" s="2">
+        <v>21</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="E23" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside1R</v>
@@ -952,15 +953,15 @@
       <c r="B24" s="2">
         <v>70</v>
       </c>
-      <c r="C24" s="2">
-        <v>23</v>
+      <c r="C24" s="4">
+        <v>22</v>
       </c>
       <c r="D24" s="2"/>
       <c r="E24" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside1R</v>
@@ -969,16 +970,14 @@
         <v>70</v>
       </c>
       <c r="C25" s="2">
-        <v>24</v>
-      </c>
-      <c r="D25" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="D25" s="2"/>
       <c r="E25" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside1R</v>
@@ -986,17 +985,17 @@
       <c r="B26" s="2">
         <v>70</v>
       </c>
-      <c r="C26" s="4">
-        <v>25</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>34</v>
+      <c r="C26" s="2">
+        <v>24</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside1R</v>
@@ -1004,80 +1003,78 @@
       <c r="B27" s="2">
         <v>70</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="4">
+        <v>25</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>wayside1R</v>
+      </c>
+      <c r="B28" s="2">
+        <v>70</v>
+      </c>
+      <c r="C28" s="2">
         <v>26</v>
       </c>
-      <c r="D27" s="2" t="s">
+      <c r="D28" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E27" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>wayside1R</v>
-      </c>
-      <c r="B28" s="2">
-        <v>30</v>
-      </c>
-      <c r="C28" s="4">
+      <c r="E28" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>wayside1R</v>
+      </c>
+      <c r="B29" s="2">
+        <v>30</v>
+      </c>
+      <c r="C29" s="4">
         <v>27</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D29" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>wayside1R</v>
-      </c>
-      <c r="B29" s="2">
-        <v>30</v>
-      </c>
-      <c r="C29" s="2">
+      <c r="E29" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B30" s="2">
+        <v>30</v>
+      </c>
+      <c r="C30" s="2">
         <v>28</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D30" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E29" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>wayside1R</v>
-      </c>
-      <c r="B30" s="2">
-        <v>30</v>
-      </c>
-      <c r="C30" s="2">
+      <c r="E30" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B31" s="2">
+        <v>30</v>
+      </c>
+      <c r="C31" s="2">
         <v>29</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>wayside1R</v>
-      </c>
-      <c r="B31" s="2">
-        <v>30</v>
-      </c>
-      <c r="C31" s="4">
-        <v>30</v>
       </c>
       <c r="D31" s="2" t="s">
         <v>23</v>
@@ -1086,15 +1083,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>44</v>
       </c>
       <c r="B32" s="2">
         <v>30</v>
       </c>
-      <c r="C32" s="2">
-        <v>31</v>
+      <c r="C32" s="4">
+        <v>30</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>23</v>
@@ -1103,106 +1100,105 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A33" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>wayside2R</v>
+    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="B33" s="2">
         <v>30</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="2">
+        <v>31</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A34" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>wayside2R</v>
+      </c>
+      <c r="B34" s="2">
+        <v>30</v>
+      </c>
+      <c r="C34" s="4">
         <v>32</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D34" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E33" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A34" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>wayside2R</v>
-      </c>
-      <c r="B34" s="2">
-        <v>30</v>
-      </c>
-      <c r="C34" s="2">
+      <c r="E34" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A35" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>wayside2R</v>
+      </c>
+      <c r="B35" s="2">
+        <v>30</v>
+      </c>
+      <c r="C35" s="2">
         <v>33</v>
       </c>
-      <c r="D34" s="2" t="s">
+      <c r="D35" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A35" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>wayside2R</v>
-      </c>
-      <c r="B35" s="2">
-        <v>30</v>
-      </c>
-      <c r="C35" s="2">
+      <c r="E35" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>wayside2R</v>
+      </c>
+      <c r="B36" s="2">
+        <v>30</v>
+      </c>
+      <c r="C36" s="2">
         <v>34</v>
       </c>
-      <c r="D35" s="2" t="s">
+      <c r="D36" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A36" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>wayside2R</v>
-      </c>
-      <c r="B36" s="2">
-        <v>30</v>
-      </c>
-      <c r="C36" s="4">
+      <c r="E36" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>wayside2R</v>
+      </c>
+      <c r="B37" s="2">
+        <v>30</v>
+      </c>
+      <c r="C37" s="4">
         <v>35</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>wayside2R</v>
-      </c>
-      <c r="B37" s="2">
-        <v>30</v>
-      </c>
-      <c r="C37" s="2">
+      <c r="D37" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>wayside2R</v>
+      </c>
+      <c r="B38" s="2">
+        <v>30</v>
+      </c>
+      <c r="C38" s="2">
         <v>36</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A38" s="2" t="str">
-        <f>A34</f>
-        <v>wayside2R</v>
-      </c>
-      <c r="B38" s="2">
-        <v>30</v>
-      </c>
-      <c r="C38" s="2">
-        <v>37</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>23</v>
@@ -1211,70 +1207,70 @@
         <v>10</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="str">
-        <f t="shared" si="0"/>
+        <f>A35</f>
         <v>wayside2R</v>
       </c>
       <c r="B39" s="2">
         <v>30</v>
       </c>
-      <c r="C39" s="4">
+      <c r="C39" s="2">
+        <v>37</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>wayside2R</v>
+      </c>
+      <c r="B40" s="2">
+        <v>30</v>
+      </c>
+      <c r="C40" s="4">
         <v>38</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D40" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E39" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A40" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>wayside2R</v>
-      </c>
-      <c r="B40" s="2">
-        <v>30</v>
-      </c>
-      <c r="C40" s="2">
+      <c r="E40" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>wayside2R</v>
+      </c>
+      <c r="B41" s="2">
+        <v>30</v>
+      </c>
+      <c r="C41" s="2">
         <v>39</v>
       </c>
-      <c r="D40" s="2" t="s">
+      <c r="D41" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E40" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>wayside2R</v>
-      </c>
-      <c r="B41" s="2">
-        <v>30</v>
-      </c>
-      <c r="C41" s="2">
+      <c r="E41" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>wayside2R</v>
+      </c>
+      <c r="B42" s="2">
+        <v>30</v>
+      </c>
+      <c r="C42" s="2">
         <v>40</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A42" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>wayside2R</v>
-      </c>
-      <c r="B42" s="2">
-        <v>30</v>
-      </c>
-      <c r="C42" s="4">
-        <v>41</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>23</v>
@@ -1283,7 +1279,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside2R</v>
@@ -1291,8 +1287,8 @@
       <c r="B43" s="2">
         <v>30</v>
       </c>
-      <c r="C43" s="2">
-        <v>42</v>
+      <c r="C43" s="4">
+        <v>41</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>23</v>
@@ -1301,7 +1297,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside2R</v>
@@ -1310,88 +1306,88 @@
         <v>30</v>
       </c>
       <c r="C44" s="2">
+        <v>42</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>wayside2R</v>
+      </c>
+      <c r="B45" s="2">
+        <v>30</v>
+      </c>
+      <c r="C45" s="2">
         <v>43</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D45" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="E44" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A45" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>wayside2R</v>
-      </c>
-      <c r="B45" s="2">
-        <v>30</v>
-      </c>
-      <c r="C45" s="4">
+      <c r="E45" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>wayside2R</v>
+      </c>
+      <c r="B46" s="2">
+        <v>30</v>
+      </c>
+      <c r="C46" s="4">
         <v>44</v>
       </c>
-      <c r="D45" s="2" t="s">
+      <c r="D46" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E45" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A46" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>wayside2R</v>
-      </c>
-      <c r="B46" s="2">
-        <v>30</v>
-      </c>
-      <c r="C46" s="2">
+      <c r="E46" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>wayside2R</v>
+      </c>
+      <c r="B47" s="2">
+        <v>30</v>
+      </c>
+      <c r="C47" s="2">
         <v>45</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D47" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="E46" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A47" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>wayside2R</v>
-      </c>
-      <c r="B47" s="2">
-        <v>30</v>
-      </c>
-      <c r="C47" s="2">
+      <c r="E47" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>wayside2R</v>
+      </c>
+      <c r="B48" s="2">
+        <v>30</v>
+      </c>
+      <c r="C48" s="2">
         <v>46</v>
       </c>
-      <c r="D47" s="2" t="s">
+      <c r="D48" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="E47" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A48" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>wayside2R</v>
-      </c>
-      <c r="B48" s="2">
-        <v>30</v>
-      </c>
-      <c r="C48" s="4">
-        <v>47</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>45</v>
       </c>
       <c r="E48" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside2R</v>
@@ -1399,17 +1395,17 @@
       <c r="B49" s="2">
         <v>30</v>
       </c>
-      <c r="C49" s="2">
-        <v>48</v>
+      <c r="C49" s="4">
+        <v>47</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>28</v>
+        <v>45</v>
       </c>
       <c r="E49" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside2R</v>
@@ -1418,30 +1414,32 @@
         <v>30</v>
       </c>
       <c r="C50" s="2">
+        <v>48</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A51" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>wayside2R</v>
+      </c>
+      <c r="B51" s="2">
+        <v>30</v>
+      </c>
+      <c r="C51" s="2">
         <v>49</v>
-      </c>
-      <c r="D50" s="2"/>
-      <c r="E50" s="2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A51" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>wayside2R</v>
-      </c>
-      <c r="B51" s="2">
-        <v>30</v>
-      </c>
-      <c r="C51" s="4">
-        <v>50</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside2R</v>
@@ -1449,15 +1447,15 @@
       <c r="B52" s="2">
         <v>30</v>
       </c>
-      <c r="C52" s="2">
-        <v>51</v>
+      <c r="C52" s="4">
+        <v>50</v>
       </c>
       <c r="D52" s="2"/>
       <c r="E52" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside2R</v>
@@ -1466,16 +1464,14 @@
         <v>30</v>
       </c>
       <c r="C53" s="2">
-        <v>52</v>
-      </c>
-      <c r="D53" s="2" t="s">
-        <v>42</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D53" s="2"/>
       <c r="E53" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside2R</v>
@@ -1483,17 +1479,17 @@
       <c r="B54" s="2">
         <v>30</v>
       </c>
-      <c r="C54" s="4">
-        <v>53</v>
+      <c r="C54" s="2">
+        <v>52</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="E54" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside2R</v>
@@ -1501,15 +1497,17 @@
       <c r="B55" s="2">
         <v>30</v>
       </c>
-      <c r="C55" s="2">
-        <v>54</v>
-      </c>
-      <c r="D55" s="2"/>
+      <c r="C55" s="4">
+        <v>53</v>
+      </c>
+      <c r="D55" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="E55" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside2R</v>
@@ -1518,14 +1516,14 @@
         <v>30</v>
       </c>
       <c r="C56" s="2">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D56" s="2"/>
       <c r="E56" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside2R</v>
@@ -1533,15 +1531,15 @@
       <c r="B57" s="2">
         <v>30</v>
       </c>
-      <c r="C57" s="4">
-        <v>56</v>
+      <c r="C57" s="2">
+        <v>55</v>
       </c>
       <c r="D57" s="2"/>
       <c r="E57" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="58" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside2R</v>
@@ -1549,15 +1547,15 @@
       <c r="B58" s="2">
         <v>30</v>
       </c>
-      <c r="C58" s="2">
-        <v>57</v>
+      <c r="C58" s="4">
+        <v>56</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="59" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside2R</v>
@@ -1566,14 +1564,14 @@
         <v>30</v>
       </c>
       <c r="C59" s="2">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D59" s="2"/>
       <c r="E59" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside2R</v>
@@ -1581,15 +1579,15 @@
       <c r="B60" s="2">
         <v>30</v>
       </c>
-      <c r="C60" s="4">
-        <v>59</v>
+      <c r="C60" s="2">
+        <v>58</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="61" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside2R</v>
@@ -1597,17 +1595,15 @@
       <c r="B61" s="2">
         <v>30</v>
       </c>
-      <c r="C61" s="2">
-        <v>60</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>29</v>
-      </c>
+      <c r="C61" s="4">
+        <v>59</v>
+      </c>
+      <c r="D61" s="2"/>
       <c r="E61" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="62" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside2R</v>
@@ -1616,46 +1612,48 @@
         <v>30</v>
       </c>
       <c r="C62" s="2">
+        <v>60</v>
+      </c>
+      <c r="D62" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>wayside2R</v>
+      </c>
+      <c r="B63" s="2">
+        <v>30</v>
+      </c>
+      <c r="C63" s="2">
         <v>61</v>
-      </c>
-      <c r="D62" s="2"/>
-      <c r="E62" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A63" s="2" t="str">
-        <f t="shared" si="0"/>
-        <v>wayside2R</v>
-      </c>
-      <c r="B63" s="2">
-        <v>30</v>
-      </c>
-      <c r="C63" s="4">
-        <v>62</v>
       </c>
       <c r="D63" s="2"/>
       <c r="E63" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside2R</v>
       </c>
       <c r="B64" s="2">
-        <v>70</v>
-      </c>
-      <c r="C64" s="2">
-        <v>63</v>
+        <v>30</v>
+      </c>
+      <c r="C64" s="4">
+        <v>62</v>
       </c>
       <c r="D64" s="2"/>
       <c r="E64" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside2R</v>
@@ -1664,14 +1662,14 @@
         <v>70</v>
       </c>
       <c r="C65" s="2">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D65" s="2"/>
       <c r="E65" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside2R</v>
@@ -1679,15 +1677,15 @@
       <c r="B66" s="2">
         <v>70</v>
       </c>
-      <c r="C66" s="4">
-        <v>65</v>
+      <c r="C66" s="2">
+        <v>64</v>
       </c>
       <c r="D66" s="2"/>
       <c r="E66" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="67" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="str">
         <f t="shared" si="0"/>
         <v>wayside2R</v>
@@ -1695,53 +1693,51 @@
       <c r="B67" s="2">
         <v>70</v>
       </c>
-      <c r="C67" s="2">
-        <v>66</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>31</v>
-      </c>
+      <c r="C67" s="4">
+        <v>65</v>
+      </c>
+      <c r="D67" s="2"/>
       <c r="E67" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="68" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="str">
-        <f t="shared" ref="A68:A77" si="1">A67</f>
+        <f t="shared" si="0"/>
         <v>wayside2R</v>
       </c>
       <c r="B68" s="2">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="C68" s="2">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D68" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="69" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" ref="A69:A78" si="1">A68</f>
         <v>wayside2R</v>
       </c>
       <c r="B69" s="2">
         <v>40</v>
       </c>
-      <c r="C69" s="4">
-        <v>68</v>
+      <c r="C69" s="2">
+        <v>67</v>
       </c>
       <c r="D69" s="2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="70" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="str">
         <f t="shared" si="1"/>
         <v>wayside2R</v>
@@ -1749,8 +1745,8 @@
       <c r="B70" s="2">
         <v>40</v>
       </c>
-      <c r="C70" s="2">
-        <v>69</v>
+      <c r="C70" s="4">
+        <v>68</v>
       </c>
       <c r="D70" s="2" t="s">
         <v>23</v>
@@ -1759,7 +1755,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="71" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="str">
         <f t="shared" si="1"/>
         <v>wayside2R</v>
@@ -1768,7 +1764,7 @@
         <v>40</v>
       </c>
       <c r="C71" s="2">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D71" s="2" t="s">
         <v>23</v>
@@ -1777,7 +1773,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="72" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="str">
         <f t="shared" si="1"/>
         <v>wayside2R</v>
@@ -1785,17 +1781,17 @@
       <c r="B72" s="2">
         <v>40</v>
       </c>
-      <c r="C72" s="4">
-        <v>71</v>
+      <c r="C72" s="2">
+        <v>70</v>
       </c>
       <c r="D72" s="2" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="73" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="str">
         <f t="shared" si="1"/>
         <v>wayside2R</v>
@@ -1803,44 +1799,42 @@
       <c r="B73" s="2">
         <v>40</v>
       </c>
-      <c r="C73" s="2">
-        <v>72</v>
+      <c r="C73" s="4">
+        <v>71</v>
       </c>
       <c r="D73" s="2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A74" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>wayside2R</v>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A74" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="B74" s="2">
         <v>40</v>
       </c>
       <c r="C74" s="2">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D74" s="2" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A75" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>wayside2R</v>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A75" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="B75" s="2">
         <v>40</v>
       </c>
-      <c r="C75" s="4">
-        <v>74</v>
+      <c r="C75" s="2">
+        <v>73</v>
       </c>
       <c r="D75" s="2" t="s">
         <v>23</v>
@@ -1849,16 +1843,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="76" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A76" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>wayside2R</v>
+    <row r="76" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A76" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="B76" s="2">
         <v>40</v>
       </c>
-      <c r="C76" s="2">
-        <v>75</v>
+      <c r="C76" s="4">
+        <v>74</v>
       </c>
       <c r="D76" s="2" t="s">
         <v>23</v>
@@ -1867,23 +1860,44 @@
         <v>21</v>
       </c>
     </row>
-    <row r="77" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A77" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>wayside2R</v>
+    <row r="77" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>43</v>
       </c>
       <c r="B77" s="2">
         <v>40</v>
       </c>
       <c r="C77" s="2">
+        <v>75</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E77" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A78" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B78" s="2">
+        <v>40</v>
+      </c>
+      <c r="C78" s="2">
         <v>76</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="D78" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E77" s="2" t="s">
+      <c r="E78" s="2" t="s">
         <v>22</v>
       </c>
+    </row>
+    <row r="79" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A79" s="2"/>
+      <c r="B79" s="2"/>
+      <c r="C79" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1892,6 +1906,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d6dbe862-8a3b-4653-8086-42db40bcd308" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004CAC5A57BCA96742B20F19105179392D" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="17a66d5eccaadda34e20e14acc443b73">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="d6dbe862-8a3b-4653-8086-42db40bcd308" xmlns:ns4="146e6ac5-474d-4643-90a9-6f9d8b40e84b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="dbc164d831e9dce8880d43a9a8186064" ns3:_="" ns4:_="">
     <xsd:import namespace="d6dbe862-8a3b-4653-8086-42db40bcd308"/>
@@ -2112,24 +2143,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D93A0EFE-AB92-443B-9453-D83E1C62E6E1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="146e6ac5-474d-4643-90a9-6f9d8b40e84b"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="d6dbe862-8a3b-4653-8086-42db40bcd308"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d6dbe862-8a3b-4653-8086-42db40bcd308" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D2159BF-AD5A-4F2B-827D-89E440D98C5C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C602C5CD-6858-4A4E-91FC-6CD4DD3D3D37}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2148,31 +2187,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4D2159BF-AD5A-4F2B-827D-89E440D98C5C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D93A0EFE-AB92-443B-9453-D83E1C62E6E1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="146e6ac5-474d-4643-90a9-6f9d8b40e84b"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="d6dbe862-8a3b-4653-8086-42db40bcd308"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{9ef9f489-e0a0-4eeb-87cc-3a526112fd0d}" enabled="0" method="" siteId="{9ef9f489-e0a0-4eeb-87cc-3a526112fd0d}" removed="1"/>

</xml_diff>